<commit_message>
Work in progress: updated drools rule.
Former-commit-id: 36520f6949449860a7aae8ac6b4b804e4d850e16
</commit_message>
<xml_diff>
--- a/acm-services/acm-service-participants/src/main/resources/rules/drools-participant-assignment-rules.xlsx
+++ b/acm-services/acm-service-participants/src/main/resources/rules/drools-participant-assignment-rules.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="5940" tabRatio="535"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="5145" tabRatio="535"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
   <si>
     <t>RuleSet</t>
   </si>
@@ -90,15 +90,9 @@
     <t>EscapeQuotes</t>
   </si>
   <si>
-    <t>$acmObject: CheckParticipantListModel</t>
-  </si>
-  <si>
     <t>objectType.equals("$param")</t>
   </si>
   <si>
-    <t>acmObject.?[objectType== 'CASE_FILE']</t>
-  </si>
-  <si>
     <t>org.springframework.expression.EvaluationContext</t>
   </si>
   <si>
@@ -124,35 +118,38 @@
   </si>
   <si>
     <t>java.util.List</t>
-  </si>
-  <si>
-    <t>participants.?[participantType == 'assignee'].isEmpty() &amp;&amp; participants.?[participantType == 'no access'].isEmpty()</t>
-  </si>
-  <si>
-    <t>participants.?[participantType == 'assignee'] == participants.?[participantType == 'no access']</t>
-  </si>
-  <si>
-    <t>eval(evalBoolean("$param", $acmObject))</t>
   </si>
   <si>
     <t>Expression 1
 Must be a Spring expression that evaluates to true or false.</t>
   </si>
   <si>
+    <t>ACTION</t>
+  </si>
+  <si>
+    <t>Add error to the list</t>
+  </si>
+  <si>
+    <t>$model: CheckParticipantListModel</t>
+  </si>
+  <si>
+    <t>eval(evalBoolean("$param", $model))</t>
+  </si>
+  <si>
+    <t>CASE_FILE</t>
+  </si>
+  <si>
+    <t>$model.addErrorMessage("$param");</t>
+  </si>
+  <si>
+    <t>Assignees cannot be on the no-access list.</t>
+  </si>
+  <si>
     <t>Expression 2
-Must be a Spring expression that evaluates to true or false.</t>
-  </si>
-  <si>
-    <t>ACTION</t>
-  </si>
-  <si>
-    <t>addError($acmObject, checkNoAccess("assignee", $acmObject))</t>
-  </si>
-  <si>
-    <t>Add error to the list</t>
-  </si>
-  <si>
-    <t>function Boolean evalBoolean(String expression, Object obj)
+Must be a Spring expression that evaluates to true or false. Check whether assignee is of not null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">function Boolean evalBoolean(String expression, Object obj)
 {
     ExpressionParser ep = new SpelExpressionParser();
     Expression exp = ep.parseExpression(expression);
@@ -160,44 +157,23 @@
     Boolean evaluated = exp.getValue(ec, obj, Boolean.class);
     return evaluated;
 }
-function void addError(CheckParticipantListModel model, String error)
+function void addErrorMessage(CheckParticipantListModel model, String error)
 {
     if(error != null &amp;&amp; !"".equals(error)){
-         if(model.getErrors() == null)
+         if(model.getErrorsList() == null)
          {
-              model.setErrors(new ArrayList());
+              model.setErrorsList(new ArrayList());
          }
-          model.getErrors().add(error);
+          model.getErrorsList().add(error);
       }
 }
-function String getAssignee(CheckParticipantListModel model){
-    String assignee = "";
-   if(model.getParticipantList() != null){
-      for(AcmParticipant ap: model.getParticipantList()){
-          if(ap.getParticipantType().equals('аssignee')){
-             assignee = ap.getParticipantLdapId();
-             break;
-          }
-      }
-    }
-     return assignee;
-}
-function String checkNoAccess(String participantType, CheckParticipantListModel model)
-{
-    if(model.getParticipantList() != null)
-    {
-         String assignee = "";
-         assignee =  getAssignee(model);
-         for(AcmParticipant ap : model.getParticipantList())
-         {
-             if (ap.getParticipantLdapId().equals(assignee) &amp;&amp;  ap.getParticipantType().equals('No Access'))
-            {
-                return "The combination of " + participantType + " and No Access is not possible";
-             } 
-         }
-    }
-    return null;
-}</t>
+</t>
+  </si>
+  <si>
+    <t>participants['No Access'].contains(participants['assignee'][0])</t>
+  </si>
+  <si>
+    <t>participants != null &amp;&amp; participants.containsKey('No Access') &amp;&amp; participants.containsKey('assignee')</t>
   </si>
 </sst>
 </file>
@@ -812,8 +788,8 @@
   </sheetPr>
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -846,7 +822,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -856,7 +832,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -866,7 +842,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -876,7 +852,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -886,7 +862,7 @@
         <v>2</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -896,7 +872,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -916,7 +892,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -926,17 +902,17 @@
         <v>2</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="360" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -980,24 +956,22 @@
         <v>7</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="4" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
-      <c r="F17" s="4" t="s">
-        <v>21</v>
-      </c>
+      <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C18" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>35</v>
@@ -1006,7 +980,7 @@
         <v>35</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="105" x14ac:dyDescent="0.25">
@@ -1020,30 +994,32 @@
         <v>10</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" t="s">
-        <v>34</v>
-      </c>
-      <c r="F20" s="13"/>
+        <v>42</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>